<commit_message>
add w2d1 ERD and SQL script intro
</commit_message>
<xml_diff>
--- a/W2D1_SQL_ERDs/MySQL.xlsx
+++ b/W2D1_SQL_ERDs/MySQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parmenion\Desktop\PYTHON_AUG_2024\W2D1_SQL_ERDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42E4C05-EC61-40D8-A1AB-F21D5463DC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753383B-4183-4F34-A2F6-4940F1319A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A01CF8EB-2C7F-4BE3-8660-8D14C1E89C62}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{A01CF8EB-2C7F-4BE3-8660-8D14C1E89C62}"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="11" r:id="rId1"/>
@@ -418,21 +418,6 @@
     <t>pizzas_and_toppings</t>
   </si>
   <si>
-    <t>bobbers</t>
-  </si>
-  <si>
-    <t>alison</t>
-  </si>
-  <si>
-    <t>123 fake st</t>
-  </si>
-  <si>
-    <t>Fkaetown</t>
-  </si>
-  <si>
-    <t>1337 N b.</t>
-  </si>
-  <si>
     <t>Utopia</t>
   </si>
   <si>
@@ -506,6 +491,21 @@
   </si>
   <si>
     <t>middle join table</t>
+  </si>
+  <si>
+    <t>bobberts</t>
+  </si>
+  <si>
+    <t>alisson</t>
+  </si>
+  <si>
+    <t>123 Fake st.</t>
+  </si>
+  <si>
+    <t>1337 N broadway</t>
+  </si>
+  <si>
+    <t>publisher</t>
   </si>
 </sst>
 </file>
@@ -720,9 +720,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2229,7 +2229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6FFDFB-76B8-4D1D-9084-B11CA6795C97}">
   <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D4" s="32" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
@@ -2294,7 +2294,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>3</v>
@@ -2303,7 +2303,7 @@
         <v>43</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>44</v>
@@ -2321,10 +2321,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F7" s="4">
         <v>45509</v>
@@ -2339,10 +2339,10 @@
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>92</v>
@@ -2363,7 +2363,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F8" s="4">
         <v>45509</v>
@@ -2378,13 +2378,13 @@
         <v>2</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="N8" s="4">
         <v>45509</v>
@@ -2426,10 +2426,10 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
@@ -2469,7 +2469,7 @@
         <v>101</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>6</v>
@@ -2481,7 +2481,7 @@
         <v>15</v>
       </c>
       <c r="R16" s="34" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="3:18" x14ac:dyDescent="0.3">
@@ -2489,10 +2489,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F17" s="4">
         <v>45509</v>
@@ -2510,10 +2510,10 @@
         <v>10</v>
       </c>
       <c r="M17" s="33" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="O17" s="4">
         <v>45509</v>
@@ -2536,7 +2536,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F18" s="4">
         <v>45509</v>
@@ -2554,10 +2554,10 @@
         <v>5</v>
       </c>
       <c r="M18" s="33" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="O18" s="4">
         <v>45509</v>
@@ -2588,10 +2588,10 @@
         <v>93</v>
       </c>
       <c r="M19" s="33" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="O19" s="4">
         <v>45509</v>
@@ -2637,7 +2637,7 @@
         <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.3">
@@ -2761,7 +2761,7 @@
         <v>45509</v>
       </c>
       <c r="J30" s="33" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="K30" s="2">
         <v>0</v>
@@ -2806,7 +2806,7 @@
         <v>38</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>6</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="36" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H36" s="39" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I36" s="40" t="s">
         <v>93</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="37" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H37" s="39" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I37" s="42" t="s">
         <v>94</v>
@@ -5642,7 +5642,7 @@
   <dimension ref="C2:K16"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5714,7 +5714,7 @@
         <v>11</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -5737,7 +5737,7 @@
         <v>99</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="K8" s="2">
         <v>2</v>
@@ -5781,10 +5781,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>14</v>
@@ -5795,13 +5795,13 @@
         <v>2</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.3">
@@ -5975,7 +5975,7 @@
   <dimension ref="C2:M12"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="M7" sqref="M7:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6048,9 +6048,6 @@
       <c r="E7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
       <c r="H7" s="2">
         <v>1</v>
       </c>
@@ -6077,9 +6074,6 @@
       <c r="E8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
       <c r="H8" s="2">
         <v>2</v>
       </c>
@@ -6105,9 +6099,6 @@
       </c>
       <c r="E9" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
       </c>
       <c r="H9" s="2">
         <v>3</v>
@@ -6135,9 +6126,6 @@
       <c r="E10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="H10" s="2">
         <v>4</v>
       </c>
@@ -6158,9 +6146,6 @@
       <c r="E11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
       <c r="H11" s="2">
         <v>5</v>
       </c>
@@ -6180,9 +6165,6 @@
       </c>
       <c r="E12" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
       </c>
       <c r="H12" s="2">
         <v>6</v>
@@ -6417,8 +6399,8 @@
   </sheetPr>
   <dimension ref="C2:J17"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6570,7 +6552,7 @@
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
@@ -6578,7 +6560,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>78</v>

</xml_diff>